<commit_message>
Update Seminario 3 - Actividades.xlsx
</commit_message>
<xml_diff>
--- a/Semestre 2023-1/Seminario 3 - Actividades.xlsx
+++ b/Semestre 2023-1/Seminario 3 - Actividades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julih\Dropbox\seminario-de-proyectos\Semestre 2023-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B23CF7-F389-4C16-B415-AEAD7A70565A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0879A819-7DEA-470B-9248-77FBCBDBFFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19380" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actividad 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Nombre</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>https://github.com/MagdaLol/AvancesProyectoTitulacion</t>
+  </si>
+  <si>
+    <t>https://github.com/petoalfredo1/Tesis</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,6 +769,9 @@
       <c r="C13" t="s">
         <v>30</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -817,7 +823,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="21.75" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -862,11 +868,12 @@
     <hyperlink ref="D10" r:id="rId2" xr:uid="{C2590E88-9615-476C-A2EB-262F8D8EBA5D}"/>
     <hyperlink ref="D3" r:id="rId3" xr:uid="{8626D2FC-9CE7-44E5-91DD-E7BD647FB8A8}"/>
     <hyperlink ref="D16" r:id="rId4" xr:uid="{EDE40B8A-078F-4D6E-BBA9-97F5DD4C4989}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{F3043B05-73A9-48D1-A255-54DDB119BE1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>